<commit_message>
opravena chyba pozice kurzoru v menu 1, změněn clock na externí, include knihoven eaglu.
</commit_message>
<xml_diff>
--- a/v3.0/odporyspinan.xlsx
+++ b/v3.0/odporyspinan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mechatronika\zdroj\v3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{027E537B-9B41-4314-8BB0-D79C6BCD0F79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F942E8-F61C-4679-BA4C-42B1DFA66F1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE4775B2-EE30-450E-B878-E336E0EC1E8E}"/>
   </bookViews>
@@ -31,10 +31,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -385,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36F6DF4-CC9C-4894-A98E-F351D1606D01}">
-  <dimension ref="B2:L17"/>
+  <dimension ref="B2:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,27 +392,27 @@
     <col min="2" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2">
         <f>1.23*(1+(G$2/F2))</f>
-        <v>3.9432352941176472</v>
+        <v>4.8476470588235294</v>
       </c>
       <c r="F2">
         <f>G3</f>
         <v>6800</v>
       </c>
       <c r="G2">
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="H2">
         <f>1/G2</f>
-        <v>6.666666666666667E-5</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3">
         <f t="shared" ref="B3:B5" si="0">1.23*(1+(G$2/F3))</f>
-        <v>13.53</v>
+        <v>17.63</v>
       </c>
       <c r="F3">
         <f>G6</f>
@@ -433,10 +429,10 @@
         <v>3.9432352941176472</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>5.5206976744186047</v>
+        <v>6.9509302325581395</v>
       </c>
       <c r="F4">
         <f>G5</f>
@@ -457,10 +453,10 @@
         <v>0.90441176470588225</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>4.8476470588235294</v>
+        <v>6.053529411764706</v>
       </c>
       <c r="F5">
         <f>G4</f>
@@ -481,13 +477,13 @@
         <v>0.67305061559507529</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>1.23*(1+(G$2/C6))</f>
-        <v>17.820697674418604</v>
+        <v>23.350930232558138</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C3:C22" si="3">1/D6</f>
+        <f t="shared" ref="C6:C16" si="3">1/D6</f>
         <v>1112.0689655172414</v>
       </c>
       <c r="D6">
@@ -509,10 +505,10 @@
         <v>2.0401846785225706</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7">
-        <f t="shared" ref="B7:B22" si="4">1.23*(1+(G$2/C7))</f>
-        <v>24.151580027359781</v>
+        <f t="shared" ref="B7:B16" si="4">1.23*(1+(G$2/C7))</f>
+        <v>31.792106703146374</v>
       </c>
       <c r="C7">
         <f t="shared" si="3"/>
@@ -530,10 +526,10 @@
         <v>0.67305061559507617</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8">
         <f t="shared" si="4"/>
-        <v>17.14764705882353</v>
+        <v>22.453529411764709</v>
       </c>
       <c r="C8">
         <f t="shared" si="3"/>
@@ -551,10 +547,10 @@
         <v>0.90441176470588225</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9">
         <f t="shared" si="4"/>
-        <v>16.243235294117643</v>
+        <v>21.247647058823528</v>
       </c>
       <c r="C9">
         <f t="shared" si="3"/>
@@ -572,10 +568,10 @@
         <v>2.7132352941176485</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10">
         <f t="shared" si="4"/>
-        <v>21.438344733242133</v>
+        <v>28.174459644322845</v>
       </c>
       <c r="C10">
         <f t="shared" si="3"/>
@@ -592,11 +588,21 @@
         <f t="shared" si="2"/>
         <v>1.6784199726402171</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>4.88</v>
+      </c>
+      <c r="R10">
+        <v>4.8476470588235294</v>
+      </c>
+      <c r="S10">
+        <f>Q10-R10</f>
+        <v>3.2352941176470473E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11">
         <f t="shared" si="4"/>
-        <v>20.533932968536252</v>
+        <v>26.968577291381667</v>
       </c>
       <c r="C11">
         <f t="shared" si="3"/>
@@ -613,11 +619,21 @@
         <f t="shared" si="2"/>
         <v>2.7132352941176432</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <v>6.93</v>
+      </c>
+      <c r="R11">
+        <v>6.9509302325581395</v>
+      </c>
+      <c r="S11">
+        <f t="shared" ref="S11:S14" si="5">Q11-R11</f>
+        <v>-2.093023255813975E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12">
         <f t="shared" si="4"/>
-        <v>19.860882352941179</v>
+        <v>26.071176470588238</v>
       </c>
       <c r="C12">
         <f t="shared" si="3"/>
@@ -634,11 +650,21 @@
         <f t="shared" si="2"/>
         <v>0.90441176470588758</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <v>6.1</v>
+      </c>
+      <c r="R12">
+        <v>6.053529411764706</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="5"/>
+        <v>4.6470588235293597E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13">
         <f t="shared" si="4"/>
-        <v>9.1383447332421337</v>
+        <v>11.774459644322848</v>
       </c>
       <c r="C13">
         <f t="shared" si="3"/>
@@ -655,11 +681,21 @@
         <f t="shared" si="2"/>
         <v>0.67305061559507351</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <v>9.44</v>
+      </c>
+      <c r="R13">
+        <v>9.6711764705882342</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="5"/>
+        <v>-0.23117647058823465</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14">
         <f t="shared" si="4"/>
-        <v>8.2339329685362515</v>
+        <v>10.568577291381668</v>
       </c>
       <c r="C14">
         <f t="shared" si="3"/>
@@ -676,11 +712,21 @@
         <f t="shared" si="2"/>
         <v>2.040184678522575</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <v>10.17</v>
+      </c>
+      <c r="R14">
+        <v>10.568577291381668</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="5"/>
+        <v>-0.39857729138166853</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15">
         <f t="shared" si="4"/>
-        <v>11.851580027359782</v>
+        <v>15.392106703146375</v>
       </c>
       <c r="C15">
         <f t="shared" si="3"/>
@@ -698,10 +744,10 @@
         <v>0.67305061559507351</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16">
         <f t="shared" si="4"/>
-        <v>7.5608823529411753</v>
+        <v>9.6711764705882342</v>
       </c>
       <c r="C16">
         <f t="shared" si="3"/>
@@ -733,7 +779,7 @@
     <sortCondition ref="K3:K17"/>
   </sortState>
   <conditionalFormatting sqref="L4:L17">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -744,6 +790,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="S10:S14">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
přidány pull-up rezistory I2C
</commit_message>
<xml_diff>
--- a/v3.0/odporyspinan.xlsx
+++ b/v3.0/odporyspinan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mechatronika\zdroj\v3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBA373A-96BC-4CB9-937B-5551E0B9F828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A99A89C-2966-4B21-AE07-AF5E78D9C236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="390" windowWidth="25440" windowHeight="15390" xr2:uid="{BE4775B2-EE30-450E-B878-E336E0EC1E8E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE4775B2-EE30-450E-B878-E336E0EC1E8E}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>LSB</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>dec</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -2287,8 +2290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36F6DF4-CC9C-4894-A98E-F351D1606D01}">
   <dimension ref="E9:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AG33" sqref="AG33"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3014,7 +3017,7 @@
         <v>21.131028529991791</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E33">
         <v>0</v>
       </c>
@@ -3022,7 +3025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E34">
         <v>1</v>
       </c>
@@ -3030,7 +3033,7 @@
         <v>1.6843266302315913</v>
       </c>
     </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E35">
         <v>2</v>
       </c>
@@ -3038,7 +3041,7 @@
         <v>2.5022109897003064</v>
       </c>
     </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E36">
         <v>4</v>
       </c>
@@ -3046,7 +3049,7 @@
         <v>4.2862964629724187</v>
       </c>
     </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E37">
         <v>3</v>
       </c>
@@ -3054,7 +3057,7 @@
         <v>4.9565376199318969</v>
       </c>
     </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E38">
         <v>5</v>
       </c>
@@ -3062,7 +3065,7 @@
         <v>6.7406230932040092</v>
       </c>
     </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E39">
         <v>6</v>
       </c>
@@ -3070,15 +3073,18 @@
         <v>7.5585074526727229</v>
       </c>
     </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E40">
         <v>7</v>
       </c>
       <c r="F40">
         <v>10.012834082904316</v>
       </c>
-    </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E41">
         <v>8</v>
       </c>
@@ -3086,7 +3092,7 @@
         <v>10.348194447087478</v>
       </c>
     </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E42">
         <v>9</v>
       </c>
@@ -3094,7 +3100,7 @@
         <v>12.802521077319071</v>
       </c>
     </row>
-    <row r="43" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E43">
         <v>10</v>
       </c>
@@ -3102,7 +3108,7 @@
         <v>13.620405436787784</v>
       </c>
     </row>
-    <row r="44" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E44">
         <v>12</v>
       </c>
@@ -3110,7 +3116,7 @@
         <v>15.404490910059899</v>
       </c>
     </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E45">
         <v>11</v>
       </c>
@@ -3118,7 +3124,7 @@
         <v>16.074732067019376</v>
       </c>
     </row>
-    <row r="46" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E46">
         <v>13</v>
       </c>
@@ -3126,7 +3132,7 @@
         <v>17.858817540291486</v>
       </c>
     </row>
-    <row r="47" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E47">
         <v>14</v>
       </c>
@@ -3134,7 +3140,7 @@
         <v>18.676701899760204</v>
       </c>
     </row>
-    <row r="48" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E48">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
zpřehledněno schéma spínaného zdroje a dokončena jeho dokumentace
</commit_message>
<xml_diff>
--- a/v3.0/odporyspinan.xlsx
+++ b/v3.0/odporyspinan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mechatronika\zdroj\v3.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE32F68-D492-4733-B9FF-4F449C7D91D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D863C92A-0E88-401C-8E7E-1FE531EDAEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="450" windowWidth="21600" windowHeight="11385" xr2:uid="{BE4775B2-EE30-450E-B878-E336E0EC1E8E}"/>
+    <workbookView xWindow="-25320" yWindow="390" windowWidth="25440" windowHeight="15390" xr2:uid="{BE4775B2-EE30-450E-B878-E336E0EC1E8E}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>LSB</t>
   </si>
@@ -114,9 +114,6 @@
     <t>1111</t>
   </si>
   <si>
-    <t>Ureg</t>
-  </si>
-  <si>
     <t>Umin</t>
   </si>
   <si>
@@ -128,12 +125,74 @@
   <si>
     <t>dec</t>
   </si>
+  <si>
+    <r>
+      <t>Zatěž [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> U out [V]</t>
+  </si>
+  <si>
+    <t>Ureg [V]</t>
+  </si>
+  <si>
+    <t>Naměřené hodnoty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Při </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uin = </t>
+  </si>
+  <si>
+    <t>24V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iout = </t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>------</t>
+  </si>
+  <si>
+    <t>Zatěž [Ω]</t>
+  </si>
+  <si>
+    <t>vstupní data</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,16 +201,49 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -159,20 +251,277 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF23F400"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -274,9 +623,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="8.0973582483938072E-2"/>
-          <c:y val="0.22651445781148452"/>
+          <c:y val="0.19528661042157125"/>
           <c:w val="0.87586141818555929"/>
-          <c:h val="0.59223353397297507"/>
+          <c:h val="0.62346135661259239"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -289,12 +638,13 @@
             <c:v>ideální hodnota</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="15875" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="bg1">
                   <a:lumMod val="65000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -442,26 +792,17 @@
             <c:v>minimální hodnota</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="00B0F0"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="x"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:srgbClr val="00B0F0"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -591,26 +932,17 @@
             <c:v>maximální hodnota</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="x"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -740,7 +1072,7 @@
             <c:v>po odečtu úbytku</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="15875" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4">
                   <a:lumMod val="75000"/>
@@ -824,57 +1156,57 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>List1!$N$14:$N$29</c:f>
+              <c:f>List1!$P$14:$P$29</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6843266302315913</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5022109897003064</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9565376199318969</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.2862964629724187</c:v>
+                  <c:v>3.5199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.7406230932040092</c:v>
+                  <c:v>2.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.5585074526727229</c:v>
+                  <c:v>5.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.012834082904316</c:v>
+                  <c:v>5.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.348194447087478</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.802521077319071</c:v>
+                  <c:v>8.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13.620405436787784</c:v>
+                  <c:v>11.3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.074732067019376</c:v>
+                  <c:v>12.2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15.404490910059899</c:v>
+                  <c:v>14.969999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17.858817540291486</c:v>
+                  <c:v>14.370000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18.676701899760204</c:v>
+                  <c:v>16.63</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>21.131028529991791</c:v>
+                  <c:v>17.399999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -887,15 +1219,15 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:idx val="5"/>
+          <c:order val="5"/>
           <c:tx>
-            <c:v>sezařené hodnoty</c:v>
+            <c:v>naměřené hodnoty</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="15875" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="92D050"/>
+                <a:srgbClr val="23F400"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -908,7 +1240,7 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="92D050"/>
+                  <a:srgbClr val="23F400"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -916,56 +1248,53 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>List1!$E$14:$E$29</c:f>
+              <c:f>List1!$J$33:$J$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
@@ -973,57 +1302,54 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>List1!$F$33:$F$48</c:f>
+              <c:f>List1!$K$33:$K$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>3.88</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6843266302315913</c:v>
+                  <c:v>4.79</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5022109897003064</c:v>
+                  <c:v>7.52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2862964629724187</c:v>
+                  <c:v>6.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9565376199318969</c:v>
+                  <c:v>9.1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.7406230932040092</c:v>
+                  <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.5585074526727229</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.012834082904316</c:v>
+                  <c:v>12.8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.348194447087478</c:v>
+                  <c:v>15.3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.802521077319071</c:v>
+                  <c:v>16.2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13.620405436787784</c:v>
+                  <c:v>18.97</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15.404490910059899</c:v>
+                  <c:v>18.37</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.074732067019376</c:v>
+                  <c:v>20.63</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17.858817540291486</c:v>
+                  <c:v>21.4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18.676701899760204</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>21.131028529991791</c:v>
+                  <c:v>22.71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1031,7 +1357,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-CF84-4A21-AE61-B9F7B376FC03}"/>
+              <c16:uniqueId val="{00000001-F870-4938-B9EC-2932012FF7C7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1045,11 +1371,179 @@
         </c:dLbls>
         <c:axId val="752654575"/>
         <c:axId val="752655823"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:v>sezařené hodnoty</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:srgbClr val="92D050"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="x"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:srgbClr val="92D050"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>List1!$E$14:$E$29</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="16"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>15</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>List1!$F$33:$F$48</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="16"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.6843266302315913</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2.5022109897003064</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4.2862964629724196</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4.9565376199318969</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6.7406230932040092</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7.5585074526727229</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>10.012834082904316</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>10.348194447087478</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>12.802521077319071</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>13.620405436787784</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>15.404490910059899</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>16.074732067019376</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>17.858817540291486</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>18.676701899760204</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>21.131028529991791</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-CF84-4A21-AE61-B9F7B376FC03}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="752654575"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="16"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1088,7 +1582,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="cs-CZ"/>
-                  <a:t>číselná hodnota</a:t>
+                  <a:t>logická hodnota</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1131,8 +1625,8 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1170,6 +1664,7 @@
         <c:crossAx val="752655823"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="752655823"/>
@@ -1222,8 +1717,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.109640085617033E-2"/>
-              <c:y val="0.12978232954151603"/>
+              <c:x val="1.1096456692913387E-2"/>
+              <c:y val="0.11193799691305334"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1257,7 +1752,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1293,7 +1788,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="752654575"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1310,10 +1805,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.6596316650215015"/>
-          <c:y val="0.55059362755629804"/>
-          <c:w val="0.29320863133977465"/>
-          <c:h val="0.26446977939596705"/>
+          <c:x val="9.6385970081714914E-2"/>
+          <c:y val="0.20476890715895599"/>
+          <c:w val="0.31593022747156607"/>
+          <c:h val="0.34325185253292601"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1959,8 +2454,8 @@
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>337456</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>82261</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>42041</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2285,79 +2780,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36F6DF4-CC9C-4894-A98E-F351D1606D01}">
-  <dimension ref="E9:O48"/>
+  <dimension ref="E3:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X37" sqref="X37"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="J9" t="s">
+    <row r="3" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
         <v>0</v>
       </c>
-      <c r="K9" t="s">
+      <c r="J3" t="s">
         <v>1</v>
       </c>
-      <c r="L9" t="s">
+      <c r="K3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
+    <row r="4" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
         <v>2</v>
       </c>
-      <c r="G10">
+      <c r="F4">
         <v>1500</v>
       </c>
-      <c r="H10">
+      <c r="G4">
         <v>3300</v>
       </c>
-      <c r="I10">
+      <c r="H4">
         <v>5100</v>
       </c>
-      <c r="J10">
+      <c r="I4">
         <v>6800</v>
       </c>
-      <c r="K10">
+      <c r="J4">
         <v>15000</v>
       </c>
-      <c r="L10">
+      <c r="K4">
         <v>1.4</v>
       </c>
     </row>
-    <row r="11" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
+    <row r="5" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="G11">
-        <f>1/(G10+$L$10)</f>
+      <c r="F5">
+        <f>1/(F4+$K$4)</f>
         <v>6.6604502464366589E-4</v>
       </c>
-      <c r="H11">
-        <f>1/(H10+$L$10)</f>
+      <c r="G5">
+        <f>1/(G4+$K$4)</f>
         <v>3.0290179923668747E-4</v>
       </c>
-      <c r="I11">
-        <f t="shared" ref="I11:J11" si="0">1/(I10+$L$10)</f>
+      <c r="H5">
+        <f>1/(H4+$K$4)</f>
         <v>1.9602462069235897E-4</v>
       </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
+      <c r="I5">
+        <f>1/(I4+$K$4)</f>
         <v>1.4702855294498193E-4</v>
       </c>
     </row>
-    <row r="13" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N10" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>34</v>
+      </c>
+      <c r="O11" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="O12" t="s">
+        <v>37</v>
+      </c>
+      <c r="P12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13" t="s">
         <v>4</v>
@@ -2372,19 +2893,25 @@
         <v>10</v>
       </c>
       <c r="K13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L13" t="s">
         <v>5</v>
       </c>
       <c r="M13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="5:15" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="O13" t="s">
+        <v>31</v>
+      </c>
+      <c r="P13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E14">
         <v>0</v>
       </c>
@@ -2406,11 +2933,18 @@
       <c r="M14">
         <v>1.23</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O14" s="5">
+        <f>1.23</f>
+        <v>1.23</v>
+      </c>
+      <c r="P14" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E15">
         <v>1</v>
       </c>
@@ -2418,7 +2952,7 @@
         <v>8</v>
       </c>
       <c r="G15">
-        <f>J11</f>
+        <f>I5</f>
         <v>1.4702855294498193E-4</v>
       </c>
       <c r="H15">
@@ -2434,27 +2968,29 @@
         <v>7141.47</v>
       </c>
       <c r="K15">
-        <f>1.23*(1+(($K$10*1.05)/H15))</f>
+        <f t="shared" ref="K15:K29" si="0">1.23*(1+(($J$4*1.05)/H15))</f>
         <v>4.228221728343855</v>
       </c>
       <c r="L15">
-        <f>1.23*(1+($K$10/I15))</f>
+        <f t="shared" ref="L15:L29" si="1">1.23*(1+($J$4/I15))</f>
         <v>3.9426768018349168</v>
       </c>
       <c r="M15">
-        <f>1.23*(1+(($K$10*0.95)/J15))</f>
+        <f t="shared" ref="M15:M29" si="2">1.23*(1+(($J$4*0.95)/J15))</f>
         <v>3.6843266302315913</v>
       </c>
-      <c r="N15">
-        <f>M15-2</f>
-        <v>1.6843266302315913</v>
-      </c>
-      <c r="O15">
-        <f>L15/(I15+K10)</f>
-        <v>1.8084512012232776E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="N15" s="7">
+        <f>$L15/3</f>
+        <v>1.3142256006116388</v>
+      </c>
+      <c r="O15" s="6">
+        <v>3.88</v>
+      </c>
+      <c r="P15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E16">
         <v>2</v>
       </c>
@@ -2462,39 +2998,45 @@
         <v>12</v>
       </c>
       <c r="G16">
-        <f>I11</f>
+        <f>H5</f>
         <v>1.9602462069235897E-4</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16:H29" si="1">I16*0.95</f>
+        <f t="shared" ref="H16:H29" si="3">I16*0.95</f>
         <v>4846.329999999999</v>
       </c>
       <c r="I16">
-        <f t="shared" ref="I16:I29" si="2">1/G16</f>
+        <f t="shared" ref="I16:I29" si="4">1/G16</f>
         <v>5101.3999999999996</v>
       </c>
       <c r="J16">
-        <f t="shared" ref="J16:J29" si="3">I16*1.05</f>
+        <f t="shared" ref="J16:J29" si="5">I16*1.05</f>
         <v>5356.47</v>
       </c>
       <c r="K16">
-        <f t="shared" ref="K16:K29" si="4">1.23*(1+(($K$10*1.05)/H16))</f>
+        <f t="shared" si="0"/>
         <v>5.227354699329184</v>
       </c>
       <c r="L16">
-        <f t="shared" ref="L16:L29" si="5">1.23*(1+($K$10/I16))</f>
+        <f t="shared" si="1"/>
         <v>4.846654251774023</v>
       </c>
       <c r="M16">
-        <f t="shared" ref="M16:M29" si="6">1.23*(1+(($K$10*0.95)/J16))</f>
+        <f t="shared" si="2"/>
         <v>4.5022109897003064</v>
       </c>
-      <c r="N16">
-        <f t="shared" ref="N16:N29" si="7">M16-2</f>
-        <v>2.5022109897003064</v>
-      </c>
-    </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N16" s="7">
+        <f t="shared" ref="N16:N29" si="6">$L16/3</f>
+        <v>1.6155514172580077</v>
+      </c>
+      <c r="O16" s="6">
+        <v>4.79</v>
+      </c>
+      <c r="P16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E17">
         <v>3</v>
       </c>
@@ -2502,39 +3044,46 @@
         <v>13</v>
       </c>
       <c r="G17">
-        <f>I11+J11</f>
+        <f>H5+I5</f>
         <v>3.430531736373409E-4</v>
       </c>
       <c r="H17">
+        <f t="shared" si="3"/>
+        <v>2769.249996807474</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="4"/>
+        <v>2914.9999966394462</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="5"/>
+        <v>3060.7499964714184</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>8.2255764276730385</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="1"/>
-        <v>2769.249996807474</v>
-      </c>
-      <c r="I17">
+        <v>7.5593310536089389</v>
+      </c>
+      <c r="M17">
         <f t="shared" si="2"/>
-        <v>2914.9999966394462</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="3"/>
-        <v>3060.7499964714184</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="4"/>
-        <v>8.2255764276730385</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="5"/>
-        <v>7.5593310536089389</v>
-      </c>
-      <c r="M17">
+        <v>6.9565376199318969</v>
+      </c>
+      <c r="N17" s="7">
         <f t="shared" si="6"/>
-        <v>6.9565376199318969</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="7"/>
-        <v>4.9565376199318969</v>
-      </c>
-    </row>
-    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
+        <v>2.5197770178696461</v>
+      </c>
+      <c r="O17" s="6">
+        <v>7.52</v>
+      </c>
+      <c r="P17" s="6">
+        <f>$K34-4</f>
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="18" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E18">
         <v>4</v>
       </c>
@@ -2542,39 +3091,46 @@
         <v>14</v>
       </c>
       <c r="G18">
-        <f>H11</f>
+        <f>G5</f>
         <v>3.0290179923668747E-4</v>
       </c>
       <c r="H18">
+        <f t="shared" si="3"/>
+        <v>3136.33</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="4"/>
+        <v>3301.4</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="5"/>
+        <v>3466.4700000000003</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>7.40680537443445</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="1"/>
-        <v>3136.33</v>
-      </c>
-      <c r="I18">
+        <v>6.8185381959168838</v>
+      </c>
+      <c r="M18">
         <f t="shared" si="2"/>
-        <v>3301.4</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="3"/>
-        <v>3466.4700000000003</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="4"/>
-        <v>7.40680537443445</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="5"/>
-        <v>6.8185381959168838</v>
-      </c>
-      <c r="M18">
+        <v>6.2862964629724187</v>
+      </c>
+      <c r="N18" s="7">
         <f t="shared" si="6"/>
-        <v>6.2862964629724187</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="7"/>
-        <v>4.2862964629724187</v>
-      </c>
-    </row>
-    <row r="19" spans="5:14" x14ac:dyDescent="0.25">
+        <v>2.2728460653056279</v>
+      </c>
+      <c r="O18" s="6">
+        <v>6.4</v>
+      </c>
+      <c r="P18" s="6">
+        <f t="shared" ref="P18:P29" si="7">$K35-4</f>
+        <v>3.5199999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E19">
         <v>5</v>
       </c>
@@ -2582,39 +3138,46 @@
         <v>15</v>
       </c>
       <c r="G19">
-        <f>J11+H11</f>
+        <f>I5+G5</f>
         <v>4.4993035218166943E-4</v>
       </c>
       <c r="H19">
+        <f t="shared" si="3"/>
+        <v>2111.4379045413148</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="4"/>
+        <v>2222.5662153066473</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="5"/>
+        <v>2333.6945260719799</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>10.405027102778307</v>
+      </c>
+      <c r="L19">
         <f t="shared" si="1"/>
-        <v>2111.4379045413148</v>
-      </c>
-      <c r="I19">
+        <v>9.5312149977518015</v>
+      </c>
+      <c r="M19">
         <f t="shared" si="2"/>
-        <v>2222.5662153066473</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="3"/>
-        <v>2333.6945260719799</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="4"/>
-        <v>10.405027102778307</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="5"/>
-        <v>9.5312149977518015</v>
-      </c>
-      <c r="M19">
+        <v>8.7406230932040092</v>
+      </c>
+      <c r="N19" s="7">
         <f t="shared" si="6"/>
-        <v>8.7406230932040092</v>
-      </c>
-      <c r="N19">
+        <v>3.1770716659172673</v>
+      </c>
+      <c r="O19" s="6">
+        <v>9.1</v>
+      </c>
+      <c r="P19" s="6">
         <f t="shared" si="7"/>
-        <v>6.7406230932040092</v>
-      </c>
-    </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
+        <v>2.4000000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E20">
         <v>6</v>
       </c>
@@ -2622,39 +3185,46 @@
         <v>17</v>
       </c>
       <c r="G20">
-        <f>H11+I11</f>
+        <f>G5+H5</f>
         <v>4.9892641992904641E-4</v>
       </c>
       <c r="H20">
+        <f t="shared" si="3"/>
+        <v>1904.0883826819631</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="4"/>
+        <v>2004.303560717856</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="5"/>
+        <v>2104.5187387537489</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>11.404160073763634</v>
+      </c>
+      <c r="L20">
         <f t="shared" si="1"/>
-        <v>1904.0883826819631</v>
-      </c>
-      <c r="I20">
+        <v>10.435192447690907</v>
+      </c>
+      <c r="M20">
         <f t="shared" si="2"/>
-        <v>2004.303560717856</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="3"/>
-        <v>2104.5187387537489</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="4"/>
-        <v>11.404160073763634</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="5"/>
-        <v>10.435192447690907</v>
-      </c>
-      <c r="M20">
+        <v>9.5585074526727229</v>
+      </c>
+      <c r="N20" s="7">
         <f t="shared" si="6"/>
-        <v>9.5585074526727229</v>
-      </c>
-      <c r="N20">
+        <v>3.4783974825636359</v>
+      </c>
+      <c r="O20" s="6">
+        <v>9.9</v>
+      </c>
+      <c r="P20" s="6">
         <f t="shared" si="7"/>
-        <v>7.5585074526727229</v>
-      </c>
-    </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E21">
         <v>7</v>
       </c>
@@ -2662,39 +3232,46 @@
         <v>16</v>
       </c>
       <c r="G21">
-        <f>H11+I11+J11</f>
+        <f>G5+H5+I5</f>
         <v>6.4595497287402832E-4</v>
       </c>
       <c r="H21">
+        <f t="shared" si="3"/>
+        <v>1470.6907445470899</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="4"/>
+        <v>1548.0955205758842</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="5"/>
+        <v>1625.5002966046784</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>14.402381802107488</v>
+      </c>
+      <c r="L21">
         <f t="shared" si="1"/>
-        <v>1470.6907445470899</v>
-      </c>
-      <c r="I21">
+        <v>13.14786924952582</v>
+      </c>
+      <c r="M21">
         <f t="shared" si="2"/>
-        <v>1548.0955205758842</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="3"/>
-        <v>1625.5002966046784</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="4"/>
-        <v>14.402381802107488</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="5"/>
-        <v>13.14786924952582</v>
-      </c>
-      <c r="M21">
+        <v>12.012834082904316</v>
+      </c>
+      <c r="N21" s="7">
         <f t="shared" si="6"/>
-        <v>12.012834082904316</v>
-      </c>
-      <c r="N21">
+        <v>4.3826230831752735</v>
+      </c>
+      <c r="O21" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="P21" s="6">
         <f t="shared" si="7"/>
-        <v>10.012834082904316</v>
-      </c>
-    </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="22" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E22">
         <v>8</v>
       </c>
@@ -2702,39 +3279,46 @@
         <v>18</v>
       </c>
       <c r="G22">
-        <f>G11</f>
+        <f>F5</f>
         <v>6.6604502464366589E-4</v>
       </c>
       <c r="H22">
+        <f t="shared" si="3"/>
+        <v>1426.33</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="4"/>
+        <v>1501.4</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="5"/>
+        <v>1576.4700000000003</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>14.812060252536231</v>
+      </c>
+      <c r="L22">
         <f t="shared" si="1"/>
-        <v>1426.33</v>
-      </c>
-      <c r="I22">
+        <v>13.518530704675635</v>
+      </c>
+      <c r="M22">
         <f t="shared" si="2"/>
-        <v>1501.4</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="3"/>
-        <v>1576.4700000000003</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="4"/>
-        <v>14.812060252536231</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="5"/>
-        <v>13.518530704675635</v>
-      </c>
-      <c r="M22">
+        <v>12.348194447087478</v>
+      </c>
+      <c r="N22" s="7">
         <f t="shared" si="6"/>
-        <v>12.348194447087478</v>
-      </c>
-      <c r="N22">
+        <v>4.5061769015585451</v>
+      </c>
+      <c r="O22" s="6">
+        <v>12.8</v>
+      </c>
+      <c r="P22" s="6">
         <f t="shared" si="7"/>
-        <v>10.348194447087478</v>
-      </c>
-    </row>
-    <row r="23" spans="5:14" x14ac:dyDescent="0.25">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="23" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E23">
         <v>9</v>
       </c>
@@ -2742,39 +3326,46 @@
         <v>19</v>
       </c>
       <c r="G23">
-        <f>G11+J11</f>
+        <f>F5+I5</f>
         <v>8.1307357758864779E-4</v>
       </c>
       <c r="H23">
+        <f t="shared" si="3"/>
+        <v>1168.4059428144722</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="4"/>
+        <v>1229.9009924362865</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="5"/>
+        <v>1291.3960420581009</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>17.810281980880085</v>
+      </c>
+      <c r="L23">
         <f t="shared" si="1"/>
-        <v>1168.4059428144722</v>
-      </c>
-      <c r="I23">
+        <v>16.23120750651055</v>
+      </c>
+      <c r="M23">
         <f t="shared" si="2"/>
-        <v>1229.9009924362865</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="3"/>
-        <v>1291.3960420581009</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="4"/>
-        <v>17.810281980880085</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="5"/>
-        <v>16.23120750651055</v>
-      </c>
-      <c r="M23">
+        <v>14.802521077319071</v>
+      </c>
+      <c r="N23" s="7">
         <f t="shared" si="6"/>
-        <v>14.802521077319071</v>
-      </c>
-      <c r="N23">
+        <v>5.4104025021701831</v>
+      </c>
+      <c r="O23" s="6">
+        <v>15.3</v>
+      </c>
+      <c r="P23" s="6">
         <f t="shared" si="7"/>
-        <v>12.802521077319071</v>
-      </c>
-    </row>
-    <row r="24" spans="5:14" x14ac:dyDescent="0.25">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E24">
         <v>10</v>
       </c>
@@ -2782,39 +3373,46 @@
         <v>20</v>
       </c>
       <c r="G24">
-        <f>G11+I11</f>
+        <f>F5+H5</f>
         <v>8.6206964533602488E-4</v>
       </c>
       <c r="H24">
+        <f t="shared" si="3"/>
+        <v>1101.9991309747379</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="4"/>
+        <v>1159.9990852365663</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="5"/>
+        <v>1217.9990394983947</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>18.809414951865413</v>
+      </c>
+      <c r="L24">
         <f t="shared" si="1"/>
-        <v>1101.9991309747379</v>
-      </c>
-      <c r="I24">
+        <v>17.135184956449656</v>
+      </c>
+      <c r="M24">
         <f t="shared" si="2"/>
-        <v>1159.9990852365663</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="3"/>
-        <v>1217.9990394983947</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="4"/>
-        <v>18.809414951865413</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="5"/>
-        <v>17.135184956449656</v>
-      </c>
-      <c r="M24">
+        <v>15.620405436787784</v>
+      </c>
+      <c r="N24" s="7">
         <f t="shared" si="6"/>
-        <v>15.620405436787784</v>
-      </c>
-      <c r="N24">
+        <v>5.7117283188165517</v>
+      </c>
+      <c r="O24" s="6">
+        <v>16.2</v>
+      </c>
+      <c r="P24" s="6">
         <f t="shared" si="7"/>
-        <v>13.620405436787784</v>
-      </c>
-    </row>
-    <row r="25" spans="5:14" x14ac:dyDescent="0.25">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="25" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E25">
         <v>11</v>
       </c>
@@ -2822,39 +3420,46 @@
         <v>21</v>
       </c>
       <c r="G25">
-        <f>G11+I11+J11</f>
+        <f>F5+H5+I5</f>
         <v>1.0090981982810068E-3</v>
       </c>
       <c r="H25">
+        <f t="shared" si="3"/>
+        <v>941.4346409678659</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="4"/>
+        <v>990.98383259775358</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="5"/>
+        <v>1040.5330242276414</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>21.807636680209264</v>
+      </c>
+      <c r="L25">
         <f t="shared" si="1"/>
-        <v>941.4346409678659</v>
-      </c>
-      <c r="I25">
+        <v>19.847861758284576</v>
+      </c>
+      <c r="M25">
         <f t="shared" si="2"/>
-        <v>990.98383259775358</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="3"/>
-        <v>1040.5330242276414</v>
-      </c>
-      <c r="K25">
-        <f t="shared" si="4"/>
-        <v>21.807636680209264</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="5"/>
-        <v>19.847861758284576</v>
-      </c>
-      <c r="M25">
+        <v>18.074732067019376</v>
+      </c>
+      <c r="N25" s="7">
         <f t="shared" si="6"/>
-        <v>18.074732067019376</v>
-      </c>
-      <c r="N25">
+        <v>6.6159539194281924</v>
+      </c>
+      <c r="O25" s="6">
+        <v>18.97</v>
+      </c>
+      <c r="P25" s="6">
         <f t="shared" si="7"/>
-        <v>16.074732067019376</v>
-      </c>
-    </row>
-    <row r="26" spans="5:14" x14ac:dyDescent="0.25">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="26" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E26">
         <v>12</v>
       </c>
@@ -2862,39 +3467,46 @@
         <v>22</v>
       </c>
       <c r="G26">
-        <f>G11+H11</f>
+        <f>F5+G5</f>
         <v>9.6894682388035331E-4</v>
       </c>
       <c r="H26">
+        <f t="shared" si="3"/>
+        <v>980.4459611060214</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="4"/>
+        <v>1032.0483801116015</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="5"/>
+        <v>1083.6507991171816</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>20.988865626970682</v>
+      </c>
+      <c r="L26">
         <f t="shared" si="1"/>
-        <v>980.4459611060214</v>
-      </c>
-      <c r="I26">
+        <v>19.10706890059252</v>
+      </c>
+      <c r="M26">
         <f t="shared" si="2"/>
-        <v>1032.0483801116015</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="3"/>
-        <v>1083.6507991171816</v>
-      </c>
-      <c r="K26">
-        <f t="shared" si="4"/>
-        <v>20.988865626970682</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="5"/>
-        <v>19.10706890059252</v>
-      </c>
-      <c r="M26">
+        <v>17.404490910059899</v>
+      </c>
+      <c r="N26" s="7">
         <f t="shared" si="6"/>
-        <v>17.404490910059899</v>
-      </c>
-      <c r="N26">
+        <v>6.3690229668641729</v>
+      </c>
+      <c r="O26" s="6">
+        <v>18.37</v>
+      </c>
+      <c r="P26" s="6">
         <f t="shared" si="7"/>
-        <v>15.404490910059899</v>
-      </c>
-    </row>
-    <row r="27" spans="5:14" x14ac:dyDescent="0.25">
+        <v>14.969999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E27">
         <v>13</v>
       </c>
@@ -2902,39 +3514,46 @@
         <v>23</v>
       </c>
       <c r="G27">
-        <f>G11+H11+J11</f>
+        <f>F5+G5+I5</f>
         <v>1.1159753768253352E-3</v>
       </c>
       <c r="H27">
+        <f t="shared" si="3"/>
+        <v>851.27326258981384</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="4"/>
+        <v>896.0771185155935</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="5"/>
+        <v>940.88097444137316</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>23.987087355314532</v>
+      </c>
+      <c r="L27">
         <f t="shared" si="1"/>
-        <v>851.27326258981384</v>
-      </c>
-      <c r="I27">
+        <v>21.819745702427436</v>
+      </c>
+      <c r="M27">
         <f t="shared" si="2"/>
-        <v>896.0771185155935</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="3"/>
-        <v>940.88097444137316</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="4"/>
-        <v>23.987087355314532</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="5"/>
-        <v>21.819745702427436</v>
-      </c>
-      <c r="M27">
+        <v>19.858817540291486</v>
+      </c>
+      <c r="N27" s="7">
         <f t="shared" si="6"/>
-        <v>19.858817540291486</v>
-      </c>
-      <c r="N27">
+        <v>7.2732485674758118</v>
+      </c>
+      <c r="O27" s="6">
+        <v>20.63</v>
+      </c>
+      <c r="P27" s="6">
         <f t="shared" si="7"/>
-        <v>17.858817540291486</v>
-      </c>
-    </row>
-    <row r="28" spans="5:14" x14ac:dyDescent="0.25">
+        <v>14.370000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E28">
         <v>14</v>
       </c>
@@ -2942,39 +3561,46 @@
         <v>24</v>
       </c>
       <c r="G28">
-        <f>G11+H11+I11</f>
+        <f>F5+G5+H5</f>
         <v>1.1649714445727123E-3</v>
       </c>
       <c r="H28">
+        <f t="shared" si="3"/>
+        <v>815.47063185607999</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="4"/>
+        <v>858.39013879587367</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="5"/>
+        <v>901.30964573566735</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>24.986220326299861</v>
+      </c>
+      <c r="L28">
         <f t="shared" si="1"/>
-        <v>815.47063185607999</v>
-      </c>
-      <c r="I28">
+        <v>22.723723152366542</v>
+      </c>
+      <c r="M28">
         <f t="shared" si="2"/>
-        <v>858.39013879587367</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="3"/>
-        <v>901.30964573566735</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="4"/>
-        <v>24.986220326299861</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="5"/>
-        <v>22.723723152366542</v>
-      </c>
-      <c r="M28">
+        <v>20.676701899760204</v>
+      </c>
+      <c r="N28" s="7">
         <f t="shared" si="6"/>
-        <v>20.676701899760204</v>
-      </c>
-      <c r="N28">
+        <v>7.5745743841221804</v>
+      </c>
+      <c r="O28" s="6">
+        <v>21.4</v>
+      </c>
+      <c r="P28" s="6">
         <f t="shared" si="7"/>
-        <v>18.676701899760204</v>
-      </c>
-    </row>
-    <row r="29" spans="5:14" x14ac:dyDescent="0.25">
+        <v>16.63</v>
+      </c>
+    </row>
+    <row r="29" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E29">
         <v>15</v>
       </c>
@@ -2982,164 +3608,500 @@
         <v>25</v>
       </c>
       <c r="G29">
-        <f>G11+H11+I11+J11</f>
+        <f>F5+G5+H5+I5</f>
         <v>1.3119999975176942E-3</v>
       </c>
       <c r="H29">
+        <f t="shared" si="3"/>
+        <v>724.08536722362908</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="4"/>
+        <v>762.19512339329378</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="5"/>
+        <v>800.30487956295849</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>27.984442054643715</v>
+      </c>
+      <c r="L29">
         <f t="shared" si="1"/>
-        <v>724.08536722362908</v>
-      </c>
-      <c r="I29">
+        <v>25.436399954201455</v>
+      </c>
+      <c r="M29">
         <f t="shared" si="2"/>
-        <v>762.19512339329378</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="3"/>
-        <v>800.30487956295849</v>
-      </c>
-      <c r="K29">
-        <f t="shared" si="4"/>
-        <v>27.984442054643715</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="5"/>
-        <v>25.436399954201455</v>
-      </c>
-      <c r="M29">
+        <v>23.131028529991791</v>
+      </c>
+      <c r="N29" s="7">
         <f t="shared" si="6"/>
-        <v>23.131028529991791</v>
-      </c>
-      <c r="N29">
+        <v>8.4787999847338185</v>
+      </c>
+      <c r="O29" s="6">
+        <v>22.71</v>
+      </c>
+      <c r="P29" s="6">
         <f t="shared" si="7"/>
-        <v>21.131028529991791</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>3.88</v>
+      </c>
+    </row>
+    <row r="34" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E34">
         <v>1</v>
       </c>
       <c r="F34">
         <v>1.6843266302315913</v>
       </c>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="K34">
+        <v>4.79</v>
+      </c>
+    </row>
+    <row r="35" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E35">
         <v>2</v>
       </c>
       <c r="F35">
         <v>2.5022109897003064</v>
       </c>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="J35">
+        <v>3</v>
+      </c>
+      <c r="K35">
+        <v>7.52</v>
+      </c>
+    </row>
+    <row r="36" spans="5:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E36">
         <v>4</v>
       </c>
       <c r="F36">
-        <v>4.2862964629724187</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
+        <v>4.2862964629724196</v>
+      </c>
+      <c r="J36">
+        <v>4</v>
+      </c>
+      <c r="K36">
+        <v>6.4</v>
+      </c>
+      <c r="M36" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="N36" s="18"/>
+      <c r="O36" s="19"/>
+    </row>
+    <row r="37" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E37">
         <v>3</v>
       </c>
       <c r="F37">
         <v>4.9565376199318969</v>
       </c>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="J37">
+        <v>5</v>
+      </c>
+      <c r="K37">
+        <v>9.1</v>
+      </c>
+      <c r="M37" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="N37" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O37" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E38">
         <v>5</v>
       </c>
       <c r="F38">
         <v>6.7406230932040092</v>
       </c>
-    </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="J38">
+        <v>6</v>
+      </c>
+      <c r="K38">
+        <v>9.9</v>
+      </c>
+      <c r="M38" s="28"/>
+      <c r="N38" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="O38" s="30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E39">
         <v>6</v>
       </c>
       <c r="F39">
         <v>7.5585074526727229</v>
       </c>
-    </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="J39">
+        <v>7</v>
+      </c>
+      <c r="K39">
+        <v>12.5</v>
+      </c>
+      <c r="M39" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="N39" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="O39" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="P39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E40">
         <v>7</v>
       </c>
       <c r="F40">
         <v>10.012834082904316</v>
       </c>
-    </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="J40">
+        <v>8</v>
+      </c>
+      <c r="K40">
+        <v>12.8</v>
+      </c>
+      <c r="M40" s="23">
+        <v>0</v>
+      </c>
+      <c r="N40" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="O40" s="25">
+        <v>1.23</v>
+      </c>
+      <c r="P40" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E41">
         <v>8</v>
       </c>
       <c r="F41">
         <v>10.348194447087478</v>
       </c>
-    </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="J41">
+        <v>9</v>
+      </c>
+      <c r="K41">
+        <v>15.3</v>
+      </c>
+      <c r="M41" s="8">
+        <v>1</v>
+      </c>
+      <c r="N41" s="9">
+        <v>1.3142256006116388</v>
+      </c>
+      <c r="O41" s="10">
+        <v>3.88</v>
+      </c>
+      <c r="P41" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E42">
         <v>9</v>
       </c>
       <c r="F42">
         <v>12.802521077319071</v>
       </c>
-    </row>
-    <row r="43" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="J42">
+        <v>10</v>
+      </c>
+      <c r="K42">
+        <v>16.2</v>
+      </c>
+      <c r="M42" s="23">
+        <v>2</v>
+      </c>
+      <c r="N42" s="26">
+        <v>1.6155514172580077</v>
+      </c>
+      <c r="O42" s="27">
+        <v>4.79</v>
+      </c>
+      <c r="P42" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E43">
         <v>10</v>
       </c>
       <c r="F43">
         <v>13.620405436787784</v>
       </c>
-    </row>
-    <row r="44" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="J43">
+        <v>11</v>
+      </c>
+      <c r="K43">
+        <v>18.97</v>
+      </c>
+      <c r="M43" s="8">
+        <v>3</v>
+      </c>
+      <c r="N43" s="9">
+        <v>2.5197770178696461</v>
+      </c>
+      <c r="O43" s="10">
+        <v>7.52</v>
+      </c>
+      <c r="P43" s="6">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="44" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E44">
         <v>12</v>
       </c>
       <c r="F44">
         <v>15.404490910059899</v>
       </c>
-    </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="J44">
+        <v>12</v>
+      </c>
+      <c r="K44">
+        <v>18.37</v>
+      </c>
+      <c r="M44" s="23">
+        <v>4</v>
+      </c>
+      <c r="N44" s="26">
+        <v>2.2728460653056279</v>
+      </c>
+      <c r="O44" s="27">
+        <v>6.4</v>
+      </c>
+      <c r="P44" s="6">
+        <v>3.5199999999999996</v>
+      </c>
+    </row>
+    <row r="45" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E45">
         <v>11</v>
       </c>
       <c r="F45">
         <v>16.074732067019376</v>
       </c>
-    </row>
-    <row r="46" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="J45">
+        <v>13</v>
+      </c>
+      <c r="K45">
+        <v>20.63</v>
+      </c>
+      <c r="M45" s="8">
+        <v>5</v>
+      </c>
+      <c r="N45" s="9">
+        <v>3.1770716659172673</v>
+      </c>
+      <c r="O45" s="10">
+        <v>9.1</v>
+      </c>
+      <c r="P45" s="6">
+        <v>2.4000000000000004</v>
+      </c>
+    </row>
+    <row r="46" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E46">
         <v>13</v>
       </c>
       <c r="F46">
         <v>17.858817540291486</v>
       </c>
-    </row>
-    <row r="47" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="J46">
+        <v>14</v>
+      </c>
+      <c r="K46">
+        <v>21.4</v>
+      </c>
+      <c r="M46" s="23">
+        <v>6</v>
+      </c>
+      <c r="N46" s="26">
+        <v>3.4783974825636359</v>
+      </c>
+      <c r="O46" s="27">
+        <v>9.9</v>
+      </c>
+      <c r="P46" s="6">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E47">
         <v>14</v>
       </c>
       <c r="F47">
         <v>18.676701899760204</v>
       </c>
-    </row>
-    <row r="48" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="J47">
+        <v>15</v>
+      </c>
+      <c r="K47">
+        <v>22.71</v>
+      </c>
+      <c r="M47" s="8">
+        <v>7</v>
+      </c>
+      <c r="N47" s="9">
+        <v>4.3826230831752735</v>
+      </c>
+      <c r="O47" s="10">
+        <v>12.5</v>
+      </c>
+      <c r="P47" s="6">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="48" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E48">
         <v>15</v>
       </c>
       <c r="F48">
         <v>21.131028529991791</v>
+      </c>
+      <c r="M48" s="23">
+        <v>8</v>
+      </c>
+      <c r="N48" s="26">
+        <v>4.5061769015585451</v>
+      </c>
+      <c r="O48" s="27">
+        <v>12.8</v>
+      </c>
+      <c r="P48" s="6">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="49" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M49" s="8">
+        <v>9</v>
+      </c>
+      <c r="N49" s="9">
+        <v>5.4104025021701831</v>
+      </c>
+      <c r="O49" s="10">
+        <v>15.3</v>
+      </c>
+      <c r="P49" s="6">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="50" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M50" s="23">
+        <v>10</v>
+      </c>
+      <c r="N50" s="26">
+        <v>5.7117283188165517</v>
+      </c>
+      <c r="O50" s="27">
+        <v>16.2</v>
+      </c>
+      <c r="P50" s="6">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="51" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M51" s="8">
+        <v>11</v>
+      </c>
+      <c r="N51" s="9">
+        <v>6.6159539194281924</v>
+      </c>
+      <c r="O51" s="10">
+        <v>18.97</v>
+      </c>
+      <c r="P51" s="6">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="52" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M52" s="23">
+        <v>12</v>
+      </c>
+      <c r="N52" s="26">
+        <v>6.3690229668641729</v>
+      </c>
+      <c r="O52" s="27">
+        <v>18.37</v>
+      </c>
+      <c r="P52" s="6">
+        <v>14.969999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M53" s="8">
+        <v>13</v>
+      </c>
+      <c r="N53" s="9">
+        <v>7.2732485674758118</v>
+      </c>
+      <c r="O53" s="10">
+        <v>20.63</v>
+      </c>
+      <c r="P53" s="6">
+        <v>14.370000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M54" s="23">
+        <v>14</v>
+      </c>
+      <c r="N54" s="26">
+        <v>7.5745743841221804</v>
+      </c>
+      <c r="O54" s="27">
+        <v>21.4</v>
+      </c>
+      <c r="P54" s="6">
+        <v>16.63</v>
+      </c>
+    </row>
+    <row r="55" spans="13:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M55" s="11">
+        <v>15</v>
+      </c>
+      <c r="N55" s="12">
+        <v>8.4787999847338185</v>
+      </c>
+      <c r="O55" s="13">
+        <v>22.71</v>
+      </c>
+      <c r="P55" s="6">
+        <v>17.399999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -3171,6 +4133,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Be my valentine From: Milan To: SOČka
</commit_message>
<xml_diff>
--- a/v3.0/odporyspinan.xlsx
+++ b/v3.0/odporyspinan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mechatronika\zdroj\v3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D863C92A-0E88-401C-8E7E-1FE531EDAEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1086AE-6C33-4E2E-9DC3-CE340DF4BF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="390" windowWidth="25440" windowHeight="15390" xr2:uid="{BE4775B2-EE30-450E-B878-E336E0EC1E8E}"/>
   </bookViews>
@@ -2782,8 +2782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36F6DF4-CC9C-4894-A98E-F351D1606D01}">
   <dimension ref="E3:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2849,6 +2849,11 @@
         <v>1.4702855294498193E-4</v>
       </c>
     </row>
+    <row r="6" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
     <row r="10" spans="5:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="N10" s="3" t="s">
         <v>33</v>
@@ -3853,7 +3858,8 @@
         <v>4.79</v>
       </c>
       <c r="P42" s="6">
-        <v>0</v>
+        <f t="shared" ref="P41:P55" si="8">O42-4</f>
+        <v>0.79</v>
       </c>
     </row>
     <row r="43" spans="5:16" x14ac:dyDescent="0.25">
@@ -3879,7 +3885,8 @@
         <v>7.52</v>
       </c>
       <c r="P43" s="6">
-        <v>0.79</v>
+        <f t="shared" si="8"/>
+        <v>3.5199999999999996</v>
       </c>
     </row>
     <row r="44" spans="5:16" x14ac:dyDescent="0.25">
@@ -3905,7 +3912,8 @@
         <v>6.4</v>
       </c>
       <c r="P44" s="6">
-        <v>3.5199999999999996</v>
+        <f t="shared" si="8"/>
+        <v>2.4000000000000004</v>
       </c>
     </row>
     <row r="45" spans="5:16" x14ac:dyDescent="0.25">
@@ -3931,7 +3939,8 @@
         <v>9.1</v>
       </c>
       <c r="P45" s="6">
-        <v>2.4000000000000004</v>
+        <f t="shared" si="8"/>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="46" spans="5:16" x14ac:dyDescent="0.25">
@@ -3957,7 +3966,8 @@
         <v>9.9</v>
       </c>
       <c r="P46" s="6">
-        <v>5.0999999999999996</v>
+        <f t="shared" si="8"/>
+        <v>5.9</v>
       </c>
     </row>
     <row r="47" spans="5:16" x14ac:dyDescent="0.25">
@@ -3983,7 +3993,8 @@
         <v>12.5</v>
       </c>
       <c r="P47" s="6">
-        <v>5.9</v>
+        <f t="shared" si="8"/>
+        <v>8.5</v>
       </c>
     </row>
     <row r="48" spans="5:16" x14ac:dyDescent="0.25">
@@ -4003,7 +4014,8 @@
         <v>12.8</v>
       </c>
       <c r="P48" s="6">
-        <v>8.5</v>
+        <f t="shared" si="8"/>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="49" spans="13:16" x14ac:dyDescent="0.25">
@@ -4017,7 +4029,8 @@
         <v>15.3</v>
       </c>
       <c r="P49" s="6">
-        <v>8.8000000000000007</v>
+        <f t="shared" si="8"/>
+        <v>11.3</v>
       </c>
     </row>
     <row r="50" spans="13:16" x14ac:dyDescent="0.25">
@@ -4031,7 +4044,8 @@
         <v>16.2</v>
       </c>
       <c r="P50" s="6">
-        <v>11.3</v>
+        <f t="shared" si="8"/>
+        <v>12.2</v>
       </c>
     </row>
     <row r="51" spans="13:16" x14ac:dyDescent="0.25">
@@ -4045,7 +4059,8 @@
         <v>18.97</v>
       </c>
       <c r="P51" s="6">
-        <v>12.2</v>
+        <f t="shared" si="8"/>
+        <v>14.969999999999999</v>
       </c>
     </row>
     <row r="52" spans="13:16" x14ac:dyDescent="0.25">
@@ -4059,7 +4074,8 @@
         <v>18.37</v>
       </c>
       <c r="P52" s="6">
-        <v>14.969999999999999</v>
+        <f t="shared" si="8"/>
+        <v>14.370000000000001</v>
       </c>
     </row>
     <row r="53" spans="13:16" x14ac:dyDescent="0.25">
@@ -4073,7 +4089,8 @@
         <v>20.63</v>
       </c>
       <c r="P53" s="6">
-        <v>14.370000000000001</v>
+        <f t="shared" si="8"/>
+        <v>16.63</v>
       </c>
     </row>
     <row r="54" spans="13:16" x14ac:dyDescent="0.25">
@@ -4087,7 +4104,8 @@
         <v>21.4</v>
       </c>
       <c r="P54" s="6">
-        <v>16.63</v>
+        <f t="shared" si="8"/>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="55" spans="13:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4101,7 +4119,8 @@
         <v>22.71</v>
       </c>
       <c r="P55" s="6">
-        <v>17.399999999999999</v>
+        <f t="shared" si="8"/>
+        <v>18.71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Opravena nekomabilita s HW stále přetrvávají chyby mód 1 a korekce napětí
</commit_message>
<xml_diff>
--- a/v3.0/odporyspinan.xlsx
+++ b/v3.0/odporyspinan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mechatronika\zdroj\v3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1086AE-6C33-4E2E-9DC3-CE340DF4BF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99ED69DE-D10B-4BBF-B2B3-046F42A79023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="390" windowWidth="25440" windowHeight="15390" xr2:uid="{BE4775B2-EE30-450E-B878-E336E0EC1E8E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE4775B2-EE30-450E-B878-E336E0EC1E8E}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -2782,8 +2782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36F6DF4-CC9C-4894-A98E-F351D1606D01}">
   <dimension ref="E3:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q50" sqref="Q50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3858,7 +3858,7 @@
         <v>4.79</v>
       </c>
       <c r="P42" s="6">
-        <f t="shared" ref="P41:P55" si="8">O42-4</f>
+        <f t="shared" ref="P42:P55" si="8">O42-4</f>
         <v>0.79</v>
       </c>
     </row>

</xml_diff>